<commit_message>
Auto commit - 11101027
</commit_message>
<xml_diff>
--- a/IM/202511_Service_Count_Report.xlsx
+++ b/IM/202511_Service_Count_Report.xlsx
@@ -4591,7 +4591,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>2025110902</v>
+        <v>2025110903</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
@@ -4630,7 +4630,7 @@
         <v>226</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P48" s="3"/>
       <c r="Q48" s="3">
@@ -4639,9 +4639,7 @@
       <c r="R48" s="3">
         <v>55821</v>
       </c>
-      <c r="S48" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
@@ -4651,15 +4649,19 @@
       <c r="Z48" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="3"/>
+      <c r="AA48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:28">
       <c r="A49" s="7">
         <v>47</v>
       </c>
       <c r="B49" s="7">
-        <v>2025110903</v>
+        <v>2025110902</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
@@ -4698,7 +4700,7 @@
         <v>226</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P49" s="7"/>
       <c r="Q49" s="7">
@@ -4707,7 +4709,9 @@
       <c r="R49" s="7">
         <v>55821</v>
       </c>
-      <c r="S49" s="7"/>
+      <c r="S49" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
@@ -4717,9 +4721,7 @@
       <c r="Z49" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AA49" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA49" s="7"/>
       <c r="AB49" s="7"/>
     </row>
     <row r="50" spans="1:28">
@@ -5271,7 +5273,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="3">
-        <v>2025110907</v>
+        <v>2025110908</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
@@ -5308,16 +5310,14 @@
       </c>
       <c r="N58" s="6"/>
       <c r="O58" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3">
         <v>52000</v>
       </c>
-      <c r="S58" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S58" s="3"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
       <c r="V58" s="3"/>
@@ -5339,7 +5339,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="7">
-        <v>2025110908</v>
+        <v>2025110907</v>
       </c>
       <c r="C59" s="7">
         <v>1</v>
@@ -5376,14 +5376,16 @@
       </c>
       <c r="N59" s="8"/>
       <c r="O59" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P59" s="7"/>
       <c r="Q59" s="7"/>
       <c r="R59" s="7">
         <v>52000</v>
       </c>
-      <c r="S59" s="7"/>
+      <c r="S59" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T59" s="7"/>
       <c r="U59" s="7"/>
       <c r="V59" s="7"/>
@@ -6405,7 +6407,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="7">
-        <v>2025110670</v>
+        <v>2025110671</v>
       </c>
       <c r="C75" s="7">
         <v>1</v>
@@ -6444,16 +6446,14 @@
         <v>282</v>
       </c>
       <c r="O75" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P75" s="7"/>
       <c r="Q75" s="7"/>
       <c r="R75" s="7">
         <v>12597</v>
       </c>
-      <c r="S75" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="S75" s="7"/>
       <c r="T75" s="7"/>
       <c r="U75" s="7"/>
       <c r="V75" s="7"/>
@@ -6463,15 +6463,19 @@
       <c r="Z75" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AA75" s="7"/>
-      <c r="AB75" s="7"/>
+      <c r="AA75" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB75" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:28">
       <c r="A76" s="3">
         <v>74</v>
       </c>
       <c r="B76" s="3">
-        <v>2025110671</v>
+        <v>2025110670</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
@@ -6510,14 +6514,16 @@
         <v>282</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
       <c r="R76" s="3">
         <v>12597</v>
       </c>
-      <c r="S76" s="3"/>
+      <c r="S76" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T76" s="3"/>
       <c r="U76" s="3"/>
       <c r="V76" s="3"/>
@@ -6527,9 +6533,7 @@
       <c r="Z76" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="AA76" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA76" s="3"/>
       <c r="AB76" s="3"/>
     </row>
     <row r="77" spans="1:28">
@@ -6739,7 +6743,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="3">
-        <v>2025110667</v>
+        <v>2025110666</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
@@ -6778,14 +6782,16 @@
         <v>288</v>
       </c>
       <c r="O80" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3">
         <v>19808</v>
       </c>
-      <c r="S80" s="3"/>
+      <c r="S80" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
@@ -6795,19 +6801,15 @@
       <c r="Z80" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="AA80" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB80" s="3">
-        <v>1</v>
-      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3"/>
     </row>
     <row r="81" spans="1:28">
       <c r="A81" s="7">
         <v>79</v>
       </c>
       <c r="B81" s="7">
-        <v>2025110666</v>
+        <v>2025110667</v>
       </c>
       <c r="C81" s="7">
         <v>1</v>
@@ -6846,16 +6848,14 @@
         <v>288</v>
       </c>
       <c r="O81" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P81" s="7"/>
       <c r="Q81" s="7"/>
       <c r="R81" s="7">
         <v>19808</v>
       </c>
-      <c r="S81" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="S81" s="7"/>
       <c r="T81" s="7"/>
       <c r="U81" s="7"/>
       <c r="V81" s="7"/>
@@ -6865,7 +6865,9 @@
       <c r="Z81" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AA81" s="7"/>
+      <c r="AA81" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="AB81" s="7"/>
     </row>
     <row r="82" spans="1:28">
@@ -7205,7 +7207,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="7">
-        <v>2025110901</v>
+        <v>2025110900</v>
       </c>
       <c r="C87" s="7">
         <v>1</v>
@@ -7244,14 +7246,16 @@
         <v>298</v>
       </c>
       <c r="O87" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P87" s="7"/>
       <c r="Q87" s="7"/>
       <c r="R87" s="7">
         <v>85670</v>
       </c>
-      <c r="S87" s="7"/>
+      <c r="S87" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="T87" s="7"/>
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
@@ -7261,19 +7265,15 @@
       <c r="Z87" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AA87" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB87" s="7">
-        <v>1</v>
-      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7"/>
     </row>
     <row r="88" spans="1:28">
       <c r="A88" s="3">
         <v>86</v>
       </c>
       <c r="B88" s="3">
-        <v>2025110900</v>
+        <v>2025110901</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
@@ -7312,16 +7312,14 @@
         <v>298</v>
       </c>
       <c r="O88" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
       <c r="R88" s="3">
         <v>85670</v>
       </c>
-      <c r="S88" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="S88" s="3"/>
       <c r="T88" s="3"/>
       <c r="U88" s="3"/>
       <c r="V88" s="3"/>
@@ -7331,7 +7329,9 @@
       <c r="Z88" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="AA88" s="3"/>
+      <c r="AA88" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="AB88" s="3"/>
     </row>
     <row r="89" spans="1:28">

</xml_diff>